<commit_message>
Atualização automática de FORO_REGIONAL_DO_PARTENON.xlsx
</commit_message>
<xml_diff>
--- a/FORO_REGIONAL_DO_PARTENON.xlsx
+++ b/FORO_REGIONAL_DO_PARTENON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49DA88FA-322B-4341-875C-21E6C55EFC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD8FD26E-ECF3-4EEF-A86C-A060BF64ECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1079,7 +1079,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{490D324A-F125-466F-920B-8F48C568C6C0}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{597BC960-6FB5-4698-A3C4-E88595EB267D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1109,10 +1109,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E39E2F-29C2-4926-9BEB-1D902C6168F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{800A0DD6-BCCB-44EC-A01B-7890AD2195BE}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +1150,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B939E8BF-7C0F-4A34-9D81-43E22AE05BEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBE8024-38AB-4145-B259-7540DE219A83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1213,7 +1213,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5D7B1E1-BA4A-4AB4-A4B8-24EFB0BB3859}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37342F08-214C-4835-B110-B033ECC2C029}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,7 +1232,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C64FD675-2FCB-C3A1-29AD-5BB5287C9034}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDEC6DD-8E87-DCE1-FFCB-3F6824D1EF4B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1281,7 +1281,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4540618D-980E-331A-80D9-5A9D4B4BAEF1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DEF927D-D1BD-612F-29FC-D9FED0A6A029}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1300,7 +1300,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F72F7F8-C728-DBBA-B851-F3855A257FD6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B027C03D-65AA-4C7F-30FE-B37D7E5E9799}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99BD964B-0E22-B194-9CF4-32469916FDF5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA07614-A472-D48F-D7B1-5DCFDEA74B51}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1362,7 +1362,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A30783-AD5C-876F-FAA1-26D15B556179}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D499CC99-A786-C119-FEF2-DA7BA0BB64F7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1405,7 +1405,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0B211A-FBF9-4FBC-AA47-F08D5CAFD553}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB69DB1-0748-4439-8F5D-099A241ED585}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1443,7 +1443,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36FFE926-10FD-4590-BB14-3688D259D5F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3499B4-3DF9-49A2-9BF4-CD145482426E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1486,7 +1486,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F3C032-D2DA-4769-8EDE-865C0AD66B92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B972D92E-9920-4CAD-B5B3-74A031B1911E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F781D9A7-B0B8-46F7-807F-E28727101D95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500FF529-B5A1-4086-8008-75E31911D056}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>